<commit_message>
Acrescimento de aba de Metricas
</commit_message>
<xml_diff>
--- a/docs/Book Cart - Suíte de Testes.xlsx
+++ b/docs/Book Cart - Suíte de Testes.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Desktop\QA\Projeto Book Cart\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Desktop\QA\Projeto Book Cart\ProjetoDeTesteBookCart\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D9F118-B581-4B7C-98A2-52FE40689C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEEAFEE-D347-46C3-9D0D-B20B8B920400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="4365" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planejamento" sheetId="4" r:id="rId1"/>
     <sheet name="Matriz de Rastreabilidade" sheetId="3" r:id="rId2"/>
     <sheet name="Roteiro de Testes" sheetId="1" r:id="rId3"/>
     <sheet name="Controle de Defeitos" sheetId="2" r:id="rId4"/>
+    <sheet name="Métricas" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Roteiro de Testes'!$A$1:$N$19</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="250">
   <si>
     <t>ID</t>
   </si>
@@ -743,6 +744,45 @@
   </si>
   <si>
     <t>/evidencias/TC-017 - Filtro de preco no limite superior.mkv</t>
+  </si>
+  <si>
+    <t>Métrica</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Casos Passaram</t>
+  </si>
+  <si>
+    <t>Casos Falharam</t>
+  </si>
+  <si>
+    <t>Taxa de Sucesso (%)</t>
+  </si>
+  <si>
+    <t>70.59</t>
+  </si>
+  <si>
+    <t>Total de User Stories</t>
+  </si>
+  <si>
+    <t>User Stories Cobertas (%)</t>
+  </si>
+  <si>
+    <t>100.0</t>
+  </si>
+  <si>
+    <t>Total de Defeitos</t>
+  </si>
+  <si>
+    <t>Defeitos Alta Severidade</t>
+  </si>
+  <si>
+    <t>Defeitos Média Severidade</t>
+  </si>
+  <si>
+    <t>Defeitos Baixa Severidade</t>
   </si>
 </sst>
 </file>
@@ -828,7 +868,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -855,6 +895,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -927,7 +979,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1016,15 +1068,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1036,9 +1079,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1063,6 +1103,31 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1448,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF2DC88-697B-4AA8-9EE2-F50916A708EE}">
   <dimension ref="A1:AD173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,10 +1524,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="44"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1653,10 +1718,10 @@
       <c r="AD6" s="14"/>
     </row>
     <row r="7" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="B7" s="48"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -1723,10 +1788,10 @@
       <c r="AD8" s="14"/>
     </row>
     <row r="9" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="B9" s="49"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1865,10 +1930,10 @@
       <c r="AD12" s="14"/>
     </row>
     <row r="13" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="B13" s="48"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -2007,10 +2072,10 @@
       <c r="AD16" s="14"/>
     </row>
     <row r="17" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="B17" s="48"/>
+      <c r="B17" s="44"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -7015,7 +7080,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7092,7 +7157,7 @@
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7221,7 +7286,7 @@
       <c r="P2" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="Q2" s="40" t="s">
+      <c r="Q2" s="37" t="s">
         <v>175</v>
       </c>
       <c r="R2" s="6" t="s">
@@ -7279,7 +7344,7 @@
       <c r="P3" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="Q3" s="44" t="s">
+      <c r="Q3" s="40" t="s">
         <v>203</v>
       </c>
       <c r="R3" s="6" t="s">
@@ -7395,7 +7460,7 @@
       <c r="P5" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="Q5" s="45" t="s">
+      <c r="Q5" s="41" t="s">
         <v>183</v>
       </c>
       <c r="R5" s="6" t="s">
@@ -7569,7 +7634,7 @@
       <c r="P8" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="Q8" s="40" t="s">
+      <c r="Q8" s="37" t="s">
         <v>199</v>
       </c>
       <c r="R8" s="6" t="s">
@@ -7627,7 +7692,7 @@
       <c r="P9" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="Q9" s="40" t="s">
+      <c r="Q9" s="37" t="s">
         <v>202</v>
       </c>
       <c r="R9" s="6" t="s">
@@ -7741,7 +7806,7 @@
       <c r="P11" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="Q11" s="40" t="s">
+      <c r="Q11" s="37" t="s">
         <v>211</v>
       </c>
       <c r="R11" s="6" t="s">
@@ -7799,7 +7864,7 @@
       <c r="P12" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="Q12" s="45" t="s">
+      <c r="Q12" s="41" t="s">
         <v>219</v>
       </c>
       <c r="R12" s="6" t="s">
@@ -7857,7 +7922,7 @@
       <c r="P13" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="Q13" s="40" t="s">
+      <c r="Q13" s="37" t="s">
         <v>218</v>
       </c>
       <c r="R13" s="6" t="s">
@@ -7928,19 +7993,19 @@
       <c r="A15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="42" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="E15" s="46" t="s">
+      <c r="E15" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="F15" s="46" t="s">
+      <c r="F15" s="42" t="s">
         <v>81</v>
       </c>
       <c r="G15" s="32" t="s">
@@ -7973,7 +8038,7 @@
       <c r="P15" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="Q15" s="40" t="s">
+      <c r="Q15" s="37" t="s">
         <v>226</v>
       </c>
       <c r="R15" s="6" t="s">
@@ -7986,19 +8051,19 @@
       <c r="A16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="42" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="E16" s="46" t="s">
+      <c r="E16" s="42" t="s">
         <v>227</v>
       </c>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="42" t="s">
         <v>229</v>
       </c>
       <c r="G16" s="32" t="s">
@@ -8031,7 +8096,7 @@
       <c r="P16" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="Q16" s="40" t="s">
+      <c r="Q16" s="37" t="s">
         <v>232</v>
       </c>
       <c r="R16" s="6" t="s">
@@ -8044,19 +8109,19 @@
       <c r="A17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="42" t="s">
         <v>76</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="46" t="s">
+      <c r="F17" s="42" t="s">
         <v>82</v>
       </c>
       <c r="G17" s="32" t="s">
@@ -8089,7 +8154,7 @@
       <c r="P17" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="Q17" s="40" t="s">
+      <c r="Q17" s="37" t="s">
         <v>235</v>
       </c>
       <c r="R17" s="6" t="s">
@@ -8102,19 +8167,19 @@
       <c r="A18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="46" t="s">
+      <c r="E18" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="46" t="s">
+      <c r="F18" s="42" t="s">
         <v>83</v>
       </c>
       <c r="G18" s="32" t="s">
@@ -8147,7 +8212,7 @@
       <c r="P18" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="Q18" s="40" t="s">
+      <c r="Q18" s="37" t="s">
         <v>236</v>
       </c>
       <c r="R18" s="6" t="s">
@@ -8157,13 +8222,13 @@
       <c r="T18" s="4"/>
     </row>
     <row r="19" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="37" t="s">
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
       <c r="G19" s="32"/>
       <c r="H19" s="7"/>
       <c r="I19" s="4"/>
@@ -8604,7 +8669,7 @@
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
-      <c r="O46" s="43"/>
+      <c r="O46" s="39"/>
       <c r="P46" s="9"/>
       <c r="Q46" s="5"/>
       <c r="R46" s="4"/>
@@ -8620,7 +8685,7 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
-      <c r="O47" s="43"/>
+      <c r="O47" s="39"/>
       <c r="P47" s="9"/>
       <c r="Q47" s="5"/>
       <c r="R47" s="4"/>
@@ -8636,7 +8701,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="43"/>
+      <c r="O48" s="39"/>
       <c r="P48" s="9"/>
       <c r="Q48" s="5"/>
       <c r="R48" s="4"/>
@@ -8652,7 +8717,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="43"/>
+      <c r="O49" s="39"/>
       <c r="P49" s="9"/>
       <c r="Q49" s="5"/>
       <c r="R49" s="4"/>
@@ -8668,7 +8733,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="43"/>
+      <c r="O50" s="39"/>
       <c r="P50" s="9"/>
       <c r="Q50" s="5"/>
       <c r="R50" s="4"/>
@@ -8684,7 +8749,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="43"/>
+      <c r="O51" s="39"/>
       <c r="P51" s="9"/>
       <c r="Q51" s="5"/>
       <c r="R51" s="4"/>
@@ -8700,7 +8765,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="43"/>
+      <c r="O52" s="39"/>
       <c r="P52" s="9"/>
       <c r="Q52" s="5"/>
       <c r="R52" s="4"/>
@@ -8716,7 +8781,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="43"/>
+      <c r="O53" s="39"/>
       <c r="P53" s="9"/>
       <c r="Q53" s="5"/>
       <c r="R53" s="4"/>
@@ -8732,7 +8797,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="43"/>
+      <c r="O54" s="39"/>
       <c r="P54" s="9"/>
       <c r="Q54" s="5"/>
       <c r="R54" s="4"/>
@@ -8748,7 +8813,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="43"/>
+      <c r="O55" s="39"/>
       <c r="P55" s="9"/>
       <c r="Q55" s="5"/>
       <c r="R55" s="4"/>
@@ -8764,7 +8829,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="43"/>
+      <c r="O56" s="39"/>
       <c r="P56" s="9"/>
       <c r="Q56" s="5"/>
       <c r="R56" s="4"/>
@@ -8780,7 +8845,7 @@
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
-      <c r="O57" s="43"/>
+      <c r="O57" s="39"/>
       <c r="P57" s="9"/>
       <c r="Q57" s="5"/>
       <c r="R57" s="4"/>
@@ -8796,7 +8861,7 @@
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
-      <c r="O58" s="43"/>
+      <c r="O58" s="39"/>
       <c r="P58" s="9"/>
       <c r="Q58" s="5"/>
       <c r="R58" s="4"/>
@@ -8812,7 +8877,7 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
-      <c r="O59" s="43"/>
+      <c r="O59" s="39"/>
       <c r="P59" s="9"/>
       <c r="Q59" s="5"/>
       <c r="R59" s="4"/>
@@ -8828,7 +8893,7 @@
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
-      <c r="O60" s="43"/>
+      <c r="O60" s="39"/>
       <c r="P60" s="9"/>
       <c r="Q60" s="5"/>
       <c r="R60" s="4"/>
@@ -8844,7 +8909,7 @@
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
-      <c r="O61" s="43"/>
+      <c r="O61" s="39"/>
       <c r="P61" s="9"/>
       <c r="Q61" s="5"/>
       <c r="R61" s="4"/>
@@ -8860,7 +8925,7 @@
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
-      <c r="O62" s="43"/>
+      <c r="O62" s="39"/>
       <c r="P62" s="9"/>
       <c r="Q62" s="5"/>
       <c r="R62" s="4"/>
@@ -8876,7 +8941,7 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
       <c r="N63" s="4"/>
-      <c r="O63" s="43"/>
+      <c r="O63" s="39"/>
       <c r="P63" s="9"/>
       <c r="Q63" s="5"/>
       <c r="R63" s="4"/>
@@ -8892,7 +8957,7 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
-      <c r="O64" s="43"/>
+      <c r="O64" s="39"/>
       <c r="P64" s="9"/>
       <c r="Q64" s="5"/>
       <c r="R64" s="4"/>
@@ -8908,7 +8973,7 @@
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
-      <c r="O65" s="43"/>
+      <c r="O65" s="39"/>
       <c r="P65" s="9"/>
       <c r="Q65" s="5"/>
       <c r="R65" s="4"/>
@@ -8924,7 +8989,7 @@
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
-      <c r="O66" s="43"/>
+      <c r="O66" s="39"/>
       <c r="P66" s="9"/>
       <c r="Q66" s="5"/>
       <c r="R66" s="4"/>
@@ -8940,7 +9005,7 @@
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
       <c r="N67" s="4"/>
-      <c r="O67" s="43"/>
+      <c r="O67" s="39"/>
       <c r="P67" s="9"/>
       <c r="Q67" s="5"/>
       <c r="R67" s="4"/>
@@ -8956,7 +9021,7 @@
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
       <c r="N68" s="4"/>
-      <c r="O68" s="43"/>
+      <c r="O68" s="39"/>
       <c r="P68" s="9"/>
       <c r="Q68" s="5"/>
       <c r="R68" s="4"/>
@@ -8972,7 +9037,7 @@
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
       <c r="N69" s="4"/>
-      <c r="O69" s="43"/>
+      <c r="O69" s="39"/>
       <c r="P69" s="9"/>
       <c r="Q69" s="5"/>
       <c r="R69" s="4"/>
@@ -8988,7 +9053,7 @@
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
       <c r="N70" s="4"/>
-      <c r="O70" s="43"/>
+      <c r="O70" s="39"/>
       <c r="P70" s="9"/>
       <c r="Q70" s="5"/>
       <c r="R70" s="4"/>
@@ -9004,7 +9069,7 @@
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
       <c r="N71" s="4"/>
-      <c r="O71" s="43"/>
+      <c r="O71" s="39"/>
       <c r="P71" s="9"/>
       <c r="Q71" s="5"/>
       <c r="R71" s="4"/>
@@ -9020,7 +9085,7 @@
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
       <c r="N72" s="4"/>
-      <c r="O72" s="43"/>
+      <c r="O72" s="39"/>
       <c r="P72" s="9"/>
       <c r="Q72" s="5"/>
       <c r="R72" s="4"/>
@@ -9036,7 +9101,7 @@
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
       <c r="N73" s="4"/>
-      <c r="O73" s="43"/>
+      <c r="O73" s="39"/>
       <c r="P73" s="9"/>
       <c r="Q73" s="5"/>
       <c r="R73" s="4"/>
@@ -9052,7 +9117,7 @@
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
       <c r="N74" s="4"/>
-      <c r="O74" s="43"/>
+      <c r="O74" s="39"/>
       <c r="P74" s="9"/>
       <c r="Q74" s="5"/>
       <c r="R74" s="4"/>
@@ -9068,7 +9133,7 @@
       <c r="L75" s="4"/>
       <c r="M75" s="4"/>
       <c r="N75" s="4"/>
-      <c r="O75" s="43"/>
+      <c r="O75" s="39"/>
       <c r="P75" s="9"/>
       <c r="Q75" s="5"/>
       <c r="R75" s="4"/>
@@ -9084,7 +9149,7 @@
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
       <c r="N76" s="4"/>
-      <c r="O76" s="43"/>
+      <c r="O76" s="39"/>
       <c r="P76" s="9"/>
       <c r="Q76" s="5"/>
       <c r="R76" s="4"/>
@@ -9100,7 +9165,7 @@
       <c r="L77" s="4"/>
       <c r="M77" s="4"/>
       <c r="N77" s="4"/>
-      <c r="O77" s="43"/>
+      <c r="O77" s="39"/>
       <c r="P77" s="9"/>
       <c r="Q77" s="5"/>
       <c r="R77" s="4"/>
@@ -9294,7 +9359,7 @@
       <c r="N89" s="4"/>
       <c r="O89" s="4"/>
       <c r="P89" s="9"/>
-      <c r="Q89" s="46"/>
+      <c r="Q89" s="42"/>
       <c r="R89" s="4"/>
       <c r="S89" s="4"/>
       <c r="T89" s="4"/>
@@ -9310,7 +9375,7 @@
       <c r="N90" s="4"/>
       <c r="O90" s="4"/>
       <c r="P90" s="9"/>
-      <c r="Q90" s="46"/>
+      <c r="Q90" s="42"/>
       <c r="R90" s="4"/>
       <c r="S90" s="4"/>
       <c r="T90" s="4"/>
@@ -9326,7 +9391,7 @@
       <c r="N91" s="4"/>
       <c r="O91" s="4"/>
       <c r="P91" s="9"/>
-      <c r="Q91" s="46"/>
+      <c r="Q91" s="42"/>
       <c r="R91" s="4"/>
       <c r="S91" s="4"/>
       <c r="T91" s="4"/>
@@ -9342,7 +9407,7 @@
       <c r="N92" s="4"/>
       <c r="O92" s="4"/>
       <c r="P92" s="9"/>
-      <c r="Q92" s="46"/>
+      <c r="Q92" s="42"/>
       <c r="R92" s="4"/>
       <c r="S92" s="4"/>
       <c r="T92" s="4"/>
@@ -9358,7 +9423,7 @@
       <c r="N93" s="4"/>
       <c r="O93" s="4"/>
       <c r="P93" s="9"/>
-      <c r="Q93" s="46"/>
+      <c r="Q93" s="42"/>
       <c r="R93" s="4"/>
       <c r="S93" s="4"/>
       <c r="T93" s="4"/>
@@ -9374,7 +9439,7 @@
       <c r="N94" s="4"/>
       <c r="O94" s="4"/>
       <c r="P94" s="9"/>
-      <c r="Q94" s="46"/>
+      <c r="Q94" s="42"/>
       <c r="R94" s="4"/>
       <c r="S94" s="4"/>
       <c r="T94" s="4"/>
@@ -9390,7 +9455,7 @@
       <c r="N95" s="4"/>
       <c r="O95" s="4"/>
       <c r="P95" s="9"/>
-      <c r="Q95" s="46"/>
+      <c r="Q95" s="42"/>
       <c r="R95" s="4"/>
       <c r="S95" s="4"/>
       <c r="T95" s="4"/>
@@ -9406,7 +9471,7 @@
       <c r="N96" s="4"/>
       <c r="O96" s="4"/>
       <c r="P96" s="9"/>
-      <c r="Q96" s="46"/>
+      <c r="Q96" s="42"/>
       <c r="R96" s="4"/>
       <c r="S96" s="4"/>
       <c r="T96" s="4"/>
@@ -9422,7 +9487,7 @@
       <c r="N97" s="4"/>
       <c r="O97" s="4"/>
       <c r="P97" s="9"/>
-      <c r="Q97" s="46"/>
+      <c r="Q97" s="42"/>
       <c r="R97" s="4"/>
       <c r="S97" s="4"/>
       <c r="T97" s="4"/>
@@ -9438,7 +9503,7 @@
       <c r="N98" s="4"/>
       <c r="O98" s="4"/>
       <c r="P98" s="9"/>
-      <c r="Q98" s="46"/>
+      <c r="Q98" s="42"/>
       <c r="R98" s="4"/>
       <c r="S98" s="4"/>
       <c r="T98" s="4"/>
@@ -9534,9 +9599,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O110"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9605,237 +9670,237 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="47" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="34">
+      <c r="F2" s="48">
         <v>45861</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="47" t="s">
         <v>166</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="47" t="s">
         <v>169</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="47" t="s">
         <v>167</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="47" t="s">
         <v>168</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="N2" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="O2" s="30" t="s">
+      <c r="O2" s="12" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+    <row r="3" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="34">
+      <c r="F3" s="48">
         <v>45862</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="47" t="s">
         <v>166</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="47" t="s">
         <v>169</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="33" t="s">
+      <c r="L3" s="47" t="s">
         <v>167</v>
       </c>
-      <c r="M3" s="33" t="s">
+      <c r="M3" s="47" t="s">
         <v>168</v>
       </c>
-      <c r="N3" s="41" t="s">
+      <c r="N3" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="O3" s="12" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F4" s="48">
         <v>45862</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="47" t="s">
         <v>166</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I4" s="33" t="s">
+      <c r="I4" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="J4" s="33" t="s">
+      <c r="J4" s="47" t="s">
         <v>169</v>
       </c>
-      <c r="K4" s="33" t="s">
+      <c r="K4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="33" t="s">
+      <c r="L4" s="47" t="s">
         <v>167</v>
       </c>
-      <c r="M4" s="33" t="s">
+      <c r="M4" s="47" t="s">
         <v>168</v>
       </c>
-      <c r="N4" s="36" t="s">
+      <c r="N4" s="50" t="s">
         <v>194</v>
       </c>
-      <c r="O4" s="30" t="s">
+      <c r="O4" s="12" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="47" t="s">
         <v>207</v>
       </c>
       <c r="B5" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="48">
         <v>45862</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="47" t="s">
         <v>166</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="J5" s="33" t="s">
+      <c r="J5" s="47" t="s">
         <v>169</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="K5" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="33" t="s">
+      <c r="L5" s="47" t="s">
         <v>167</v>
       </c>
-      <c r="M5" s="33" t="s">
+      <c r="M5" s="47" t="s">
         <v>168</v>
       </c>
-      <c r="N5" s="36" t="s">
+      <c r="N5" s="50" t="s">
         <v>209</v>
       </c>
-      <c r="O5" s="30" t="s">
+      <c r="O5" s="12" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+    <row r="6" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
         <v>221</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="48">
         <v>45863</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="47" t="s">
         <v>166</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I6" s="33" t="s">
+      <c r="I6" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="47" t="s">
         <v>169</v>
       </c>
-      <c r="K6" s="33" t="s">
+      <c r="K6" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="47" t="s">
         <v>167</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="M6" s="47" t="s">
         <v>168</v>
       </c>
-      <c r="N6" s="36" t="s">
+      <c r="N6" s="50" t="s">
         <v>225</v>
       </c>
-      <c r="O6" s="30" t="s">
+      <c r="O6" s="12" t="s">
         <v>170</v>
       </c>
     </row>
@@ -9853,7 +9918,7 @@
       <c r="K7" s="33"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="42"/>
+      <c r="N7" s="38"/>
       <c r="O7" s="30"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -9870,7 +9935,7 @@
       <c r="K8" s="33"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="42"/>
+      <c r="N8" s="38"/>
       <c r="O8" s="30"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -9887,7 +9952,7 @@
       <c r="K9" s="33"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="42"/>
+      <c r="N9" s="38"/>
       <c r="O9" s="30"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -9904,7 +9969,7 @@
       <c r="K10" s="33"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="42"/>
+      <c r="N10" s="38"/>
       <c r="O10" s="30"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -9921,7 +9986,7 @@
       <c r="K11" s="33"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="42"/>
+      <c r="N11" s="38"/>
       <c r="O11" s="30"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -9938,7 +10003,7 @@
       <c r="K12" s="33"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="42"/>
+      <c r="N12" s="38"/>
       <c r="O12" s="30"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -9955,7 +10020,7 @@
       <c r="K13" s="33"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="42"/>
+      <c r="N13" s="38"/>
       <c r="O13" s="30"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -9972,7 +10037,7 @@
       <c r="K14" s="33"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="42"/>
+      <c r="N14" s="38"/>
       <c r="O14" s="30"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -9989,7 +10054,7 @@
       <c r="K15" s="33"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="42"/>
+      <c r="N15" s="38"/>
       <c r="O15" s="30"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -10006,7 +10071,7 @@
       <c r="K16" s="33"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="42"/>
+      <c r="N16" s="38"/>
       <c r="O16" s="30"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -10023,7 +10088,7 @@
       <c r="K17" s="33"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="42"/>
+      <c r="N17" s="38"/>
       <c r="O17" s="30"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -10040,7 +10105,7 @@
       <c r="K18" s="33"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="42"/>
+      <c r="N18" s="38"/>
       <c r="O18" s="30"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -10057,7 +10122,7 @@
       <c r="K19" s="33"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="42"/>
+      <c r="N19" s="38"/>
       <c r="O19" s="30"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -10074,7 +10139,7 @@
       <c r="K20" s="33"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="N20" s="42"/>
+      <c r="N20" s="38"/>
       <c r="O20" s="30"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -10091,7 +10156,7 @@
       <c r="K21" s="33"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="N21" s="42"/>
+      <c r="N21" s="38"/>
       <c r="O21" s="30"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -10108,7 +10173,7 @@
       <c r="K22" s="33"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-      <c r="N22" s="42"/>
+      <c r="N22" s="38"/>
       <c r="O22" s="30"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -10125,7 +10190,7 @@
       <c r="K23" s="33"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-      <c r="N23" s="42"/>
+      <c r="N23" s="38"/>
       <c r="O23" s="30"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -10142,7 +10207,7 @@
       <c r="K24" s="33"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-      <c r="N24" s="42"/>
+      <c r="N24" s="38"/>
       <c r="O24" s="30"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -10159,7 +10224,7 @@
       <c r="K25" s="33"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-      <c r="N25" s="42"/>
+      <c r="N25" s="38"/>
       <c r="O25" s="30"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -10176,7 +10241,7 @@
       <c r="K26" s="33"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-      <c r="N26" s="42"/>
+      <c r="N26" s="38"/>
       <c r="O26" s="30"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -10193,7 +10258,7 @@
       <c r="K27" s="33"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
-      <c r="N27" s="42"/>
+      <c r="N27" s="38"/>
       <c r="O27" s="30"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -10210,7 +10275,7 @@
       <c r="K28" s="33"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-      <c r="N28" s="42"/>
+      <c r="N28" s="38"/>
       <c r="O28" s="30"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -10227,7 +10292,7 @@
       <c r="K29" s="33"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-      <c r="N29" s="42"/>
+      <c r="N29" s="38"/>
       <c r="O29" s="30"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -10244,7 +10309,7 @@
       <c r="K30" s="33"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
-      <c r="N30" s="42"/>
+      <c r="N30" s="38"/>
       <c r="O30" s="30"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -10261,7 +10326,7 @@
       <c r="K31" s="33"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
-      <c r="N31" s="42"/>
+      <c r="N31" s="38"/>
       <c r="O31" s="30"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -10278,7 +10343,7 @@
       <c r="K32" s="33"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
-      <c r="N32" s="42"/>
+      <c r="N32" s="38"/>
       <c r="O32" s="30"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -10295,7 +10360,7 @@
       <c r="K33" s="33"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
-      <c r="N33" s="42"/>
+      <c r="N33" s="38"/>
       <c r="O33" s="30"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -10312,7 +10377,7 @@
       <c r="K34" s="33"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
-      <c r="N34" s="42"/>
+      <c r="N34" s="38"/>
       <c r="O34" s="30"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -10329,7 +10394,7 @@
       <c r="K35" s="33"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
-      <c r="N35" s="42"/>
+      <c r="N35" s="38"/>
       <c r="O35" s="30"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -10346,7 +10411,7 @@
       <c r="K36" s="33"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
-      <c r="N36" s="42"/>
+      <c r="N36" s="38"/>
       <c r="O36" s="30"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -10363,7 +10428,7 @@
       <c r="K37" s="33"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
-      <c r="N37" s="42"/>
+      <c r="N37" s="38"/>
       <c r="O37" s="30"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -10380,7 +10445,7 @@
       <c r="K38" s="33"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
-      <c r="N38" s="42"/>
+      <c r="N38" s="38"/>
       <c r="O38" s="30"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -10397,7 +10462,7 @@
       <c r="K39" s="33"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
-      <c r="N39" s="42"/>
+      <c r="N39" s="38"/>
       <c r="O39" s="30"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -10414,7 +10479,7 @@
       <c r="K40" s="33"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
-      <c r="N40" s="42"/>
+      <c r="N40" s="38"/>
       <c r="O40" s="30"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -10431,7 +10496,7 @@
       <c r="K41" s="33"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
-      <c r="N41" s="42"/>
+      <c r="N41" s="38"/>
       <c r="O41" s="30"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -10448,7 +10513,7 @@
       <c r="K42" s="33"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
-      <c r="N42" s="42"/>
+      <c r="N42" s="38"/>
       <c r="O42" s="30"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -10465,7 +10530,7 @@
       <c r="K43" s="33"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
-      <c r="N43" s="42"/>
+      <c r="N43" s="38"/>
       <c r="O43" s="30"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -10482,7 +10547,7 @@
       <c r="K44" s="33"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
-      <c r="N44" s="42"/>
+      <c r="N44" s="38"/>
       <c r="O44" s="30"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -10499,7 +10564,7 @@
       <c r="K45" s="33"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
-      <c r="N45" s="42"/>
+      <c r="N45" s="38"/>
       <c r="O45" s="30"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
@@ -10516,7 +10581,7 @@
       <c r="K46" s="33"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
-      <c r="N46" s="42"/>
+      <c r="N46" s="38"/>
       <c r="O46" s="30"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
@@ -10533,7 +10598,7 @@
       <c r="K47" s="33"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
-      <c r="N47" s="42"/>
+      <c r="N47" s="38"/>
       <c r="O47" s="30"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
@@ -10550,7 +10615,7 @@
       <c r="K48" s="33"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
-      <c r="N48" s="42"/>
+      <c r="N48" s="38"/>
       <c r="O48" s="30"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -10567,7 +10632,7 @@
       <c r="K49" s="33"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
-      <c r="N49" s="42"/>
+      <c r="N49" s="38"/>
       <c r="O49" s="30"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -10584,7 +10649,7 @@
       <c r="K50" s="33"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
-      <c r="N50" s="42"/>
+      <c r="N50" s="38"/>
       <c r="O50" s="30"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -10601,7 +10666,7 @@
       <c r="K51" s="33"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
-      <c r="N51" s="42"/>
+      <c r="N51" s="38"/>
       <c r="O51" s="30"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -10618,7 +10683,7 @@
       <c r="K52" s="33"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
-      <c r="N52" s="42"/>
+      <c r="N52" s="38"/>
       <c r="O52" s="30"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -10635,7 +10700,7 @@
       <c r="K53" s="33"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
-      <c r="N53" s="42"/>
+      <c r="N53" s="38"/>
       <c r="O53" s="30"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -10652,7 +10717,7 @@
       <c r="K54" s="33"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
-      <c r="N54" s="42"/>
+      <c r="N54" s="38"/>
       <c r="O54" s="30"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -10669,467 +10734,467 @@
       <c r="K55" s="33"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
-      <c r="N55" s="42"/>
+      <c r="N55" s="38"/>
       <c r="O55" s="30"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="38"/>
-      <c r="B56" s="37"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="38"/>
-      <c r="G56" s="38"/>
-      <c r="K56" s="38"/>
-      <c r="N56" s="39"/>
-      <c r="O56" s="37"/>
+      <c r="A56" s="35"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
+      <c r="G56" s="35"/>
+      <c r="K56" s="35"/>
+      <c r="N56" s="36"/>
+      <c r="O56" s="34"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="38"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="38"/>
-      <c r="D57" s="38"/>
-      <c r="E57" s="38"/>
-      <c r="G57" s="38"/>
-      <c r="K57" s="38"/>
-      <c r="N57" s="39"/>
-      <c r="O57" s="37"/>
+      <c r="A57" s="35"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="35"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="35"/>
+      <c r="G57" s="35"/>
+      <c r="K57" s="35"/>
+      <c r="N57" s="36"/>
+      <c r="O57" s="34"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="37"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="38"/>
-      <c r="G58" s="38"/>
-      <c r="K58" s="38"/>
-      <c r="N58" s="39"/>
-      <c r="O58" s="37"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="G58" s="35"/>
+      <c r="K58" s="35"/>
+      <c r="N58" s="36"/>
+      <c r="O58" s="34"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="37"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="38"/>
-      <c r="E59" s="38"/>
-      <c r="G59" s="38"/>
-      <c r="K59" s="38"/>
-      <c r="N59" s="39"/>
-      <c r="O59" s="37"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="G59" s="35"/>
+      <c r="K59" s="35"/>
+      <c r="N59" s="36"/>
+      <c r="O59" s="34"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="37"/>
-      <c r="C60" s="38"/>
-      <c r="D60" s="38"/>
-      <c r="E60" s="38"/>
-      <c r="G60" s="38"/>
-      <c r="K60" s="38"/>
-      <c r="N60" s="39"/>
-      <c r="O60" s="37"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="35"/>
+      <c r="E60" s="35"/>
+      <c r="G60" s="35"/>
+      <c r="K60" s="35"/>
+      <c r="N60" s="36"/>
+      <c r="O60" s="34"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="37"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="38"/>
-      <c r="E61" s="38"/>
-      <c r="G61" s="38"/>
-      <c r="K61" s="38"/>
-      <c r="N61" s="39"/>
-      <c r="O61" s="37"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
+      <c r="G61" s="35"/>
+      <c r="K61" s="35"/>
+      <c r="N61" s="36"/>
+      <c r="O61" s="34"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
-      <c r="E62" s="38"/>
-      <c r="G62" s="38"/>
-      <c r="K62" s="38"/>
-      <c r="N62" s="39"/>
-      <c r="O62" s="37"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
+      <c r="G62" s="35"/>
+      <c r="K62" s="35"/>
+      <c r="N62" s="36"/>
+      <c r="O62" s="34"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
-      <c r="E63" s="38"/>
-      <c r="G63" s="38"/>
-      <c r="K63" s="38"/>
-      <c r="N63" s="39"/>
-      <c r="O63" s="37"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
+      <c r="G63" s="35"/>
+      <c r="K63" s="35"/>
+      <c r="N63" s="36"/>
+      <c r="O63" s="34"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
-      <c r="E64" s="38"/>
-      <c r="G64" s="38"/>
-      <c r="K64" s="38"/>
-      <c r="N64" s="39"/>
-      <c r="O64" s="37"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="35"/>
+      <c r="G64" s="35"/>
+      <c r="K64" s="35"/>
+      <c r="N64" s="36"/>
+      <c r="O64" s="34"/>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="38"/>
-      <c r="E65" s="38"/>
-      <c r="G65" s="38"/>
-      <c r="K65" s="38"/>
-      <c r="N65" s="39"/>
-      <c r="O65" s="37"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="35"/>
+      <c r="G65" s="35"/>
+      <c r="K65" s="35"/>
+      <c r="N65" s="36"/>
+      <c r="O65" s="34"/>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="38"/>
-      <c r="G66" s="38"/>
-      <c r="K66" s="38"/>
-      <c r="N66" s="39"/>
-      <c r="O66" s="37"/>
+      <c r="C66" s="35"/>
+      <c r="D66" s="35"/>
+      <c r="E66" s="35"/>
+      <c r="G66" s="35"/>
+      <c r="K66" s="35"/>
+      <c r="N66" s="36"/>
+      <c r="O66" s="34"/>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
-      <c r="C67" s="38"/>
-      <c r="D67" s="38"/>
-      <c r="E67" s="38"/>
-      <c r="G67" s="38"/>
-      <c r="K67" s="38"/>
-      <c r="N67" s="39"/>
-      <c r="O67" s="37"/>
+      <c r="C67" s="35"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="35"/>
+      <c r="G67" s="35"/>
+      <c r="K67" s="35"/>
+      <c r="N67" s="36"/>
+      <c r="O67" s="34"/>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="38"/>
-      <c r="E68" s="38"/>
-      <c r="G68" s="38"/>
-      <c r="K68" s="38"/>
-      <c r="N68" s="39"/>
-      <c r="O68" s="37"/>
+      <c r="C68" s="35"/>
+      <c r="D68" s="35"/>
+      <c r="E68" s="35"/>
+      <c r="G68" s="35"/>
+      <c r="K68" s="35"/>
+      <c r="N68" s="36"/>
+      <c r="O68" s="34"/>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
-      <c r="C69" s="38"/>
-      <c r="D69" s="38"/>
-      <c r="E69" s="38"/>
-      <c r="G69" s="38"/>
-      <c r="K69" s="38"/>
-      <c r="N69" s="39"/>
-      <c r="O69" s="37"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
+      <c r="E69" s="35"/>
+      <c r="G69" s="35"/>
+      <c r="K69" s="35"/>
+      <c r="N69" s="36"/>
+      <c r="O69" s="34"/>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
-      <c r="C70" s="38"/>
-      <c r="D70" s="38"/>
-      <c r="E70" s="38"/>
-      <c r="G70" s="38"/>
-      <c r="K70" s="38"/>
-      <c r="N70" s="39"/>
-      <c r="O70" s="37"/>
+      <c r="C70" s="35"/>
+      <c r="D70" s="35"/>
+      <c r="E70" s="35"/>
+      <c r="G70" s="35"/>
+      <c r="K70" s="35"/>
+      <c r="N70" s="36"/>
+      <c r="O70" s="34"/>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
-      <c r="C71" s="38"/>
-      <c r="D71" s="38"/>
-      <c r="E71" s="38"/>
-      <c r="G71" s="38"/>
-      <c r="K71" s="38"/>
-      <c r="N71" s="39"/>
-      <c r="O71" s="37"/>
+      <c r="C71" s="35"/>
+      <c r="D71" s="35"/>
+      <c r="E71" s="35"/>
+      <c r="G71" s="35"/>
+      <c r="K71" s="35"/>
+      <c r="N71" s="36"/>
+      <c r="O71" s="34"/>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="38"/>
-      <c r="E72" s="38"/>
-      <c r="G72" s="38"/>
-      <c r="K72" s="38"/>
-      <c r="N72" s="39"/>
-      <c r="O72" s="37"/>
+      <c r="C72" s="35"/>
+      <c r="D72" s="35"/>
+      <c r="E72" s="35"/>
+      <c r="G72" s="35"/>
+      <c r="K72" s="35"/>
+      <c r="N72" s="36"/>
+      <c r="O72" s="34"/>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B73" s="2"/>
-      <c r="C73" s="38"/>
-      <c r="D73" s="38"/>
-      <c r="E73" s="38"/>
-      <c r="G73" s="38"/>
-      <c r="K73" s="38"/>
-      <c r="N73" s="39"/>
-      <c r="O73" s="37"/>
+      <c r="C73" s="35"/>
+      <c r="D73" s="35"/>
+      <c r="E73" s="35"/>
+      <c r="G73" s="35"/>
+      <c r="K73" s="35"/>
+      <c r="N73" s="36"/>
+      <c r="O73" s="34"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
-      <c r="C74" s="38"/>
-      <c r="D74" s="38"/>
-      <c r="E74" s="38"/>
-      <c r="G74" s="38"/>
-      <c r="K74" s="38"/>
-      <c r="N74" s="39"/>
-      <c r="O74" s="37"/>
+      <c r="C74" s="35"/>
+      <c r="D74" s="35"/>
+      <c r="E74" s="35"/>
+      <c r="G74" s="35"/>
+      <c r="K74" s="35"/>
+      <c r="N74" s="36"/>
+      <c r="O74" s="34"/>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B75" s="2"/>
-      <c r="C75" s="38"/>
-      <c r="D75" s="38"/>
-      <c r="E75" s="38"/>
-      <c r="G75" s="38"/>
-      <c r="K75" s="38"/>
-      <c r="N75" s="39"/>
+      <c r="C75" s="35"/>
+      <c r="D75" s="35"/>
+      <c r="E75" s="35"/>
+      <c r="G75" s="35"/>
+      <c r="K75" s="35"/>
+      <c r="N75" s="36"/>
       <c r="O75" s="2"/>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B76" s="2"/>
-      <c r="C76" s="38"/>
-      <c r="D76" s="38"/>
-      <c r="E76" s="38"/>
-      <c r="G76" s="38"/>
-      <c r="K76" s="38"/>
-      <c r="N76" s="39"/>
+      <c r="C76" s="35"/>
+      <c r="D76" s="35"/>
+      <c r="E76" s="35"/>
+      <c r="G76" s="35"/>
+      <c r="K76" s="35"/>
+      <c r="N76" s="36"/>
       <c r="O76" s="2"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B77" s="2"/>
-      <c r="C77" s="38"/>
-      <c r="D77" s="38"/>
-      <c r="E77" s="38"/>
-      <c r="G77" s="38"/>
-      <c r="K77" s="38"/>
-      <c r="N77" s="39"/>
+      <c r="C77" s="35"/>
+      <c r="D77" s="35"/>
+      <c r="E77" s="35"/>
+      <c r="G77" s="35"/>
+      <c r="K77" s="35"/>
+      <c r="N77" s="36"/>
       <c r="O77" s="2"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B78" s="2"/>
-      <c r="C78" s="38"/>
-      <c r="D78" s="38"/>
-      <c r="E78" s="38"/>
-      <c r="G78" s="38"/>
-      <c r="K78" s="38"/>
-      <c r="N78" s="39"/>
+      <c r="C78" s="35"/>
+      <c r="D78" s="35"/>
+      <c r="E78" s="35"/>
+      <c r="G78" s="35"/>
+      <c r="K78" s="35"/>
+      <c r="N78" s="36"/>
       <c r="O78" s="2"/>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B79" s="2"/>
-      <c r="C79" s="38"/>
-      <c r="D79" s="38"/>
-      <c r="E79" s="38"/>
-      <c r="G79" s="38"/>
-      <c r="K79" s="38"/>
-      <c r="N79" s="39"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="35"/>
+      <c r="E79" s="35"/>
+      <c r="G79" s="35"/>
+      <c r="K79" s="35"/>
+      <c r="N79" s="36"/>
       <c r="O79" s="2"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B80" s="2"/>
-      <c r="C80" s="38"/>
-      <c r="D80" s="38"/>
-      <c r="E80" s="38"/>
-      <c r="G80" s="38"/>
-      <c r="K80" s="38"/>
-      <c r="N80" s="39"/>
+      <c r="C80" s="35"/>
+      <c r="D80" s="35"/>
+      <c r="E80" s="35"/>
+      <c r="G80" s="35"/>
+      <c r="K80" s="35"/>
+      <c r="N80" s="36"/>
       <c r="O80" s="2"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B81" s="2"/>
-      <c r="C81" s="38"/>
-      <c r="D81" s="38"/>
-      <c r="E81" s="38"/>
-      <c r="G81" s="38"/>
-      <c r="K81" s="38"/>
-      <c r="N81" s="39"/>
+      <c r="C81" s="35"/>
+      <c r="D81" s="35"/>
+      <c r="E81" s="35"/>
+      <c r="G81" s="35"/>
+      <c r="K81" s="35"/>
+      <c r="N81" s="36"/>
       <c r="O81" s="2"/>
     </row>
     <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B82" s="2"/>
-      <c r="C82" s="38"/>
-      <c r="E82" s="38"/>
-      <c r="G82" s="38"/>
-      <c r="K82" s="38"/>
-      <c r="N82" s="39"/>
+      <c r="C82" s="35"/>
+      <c r="E82" s="35"/>
+      <c r="G82" s="35"/>
+      <c r="K82" s="35"/>
+      <c r="N82" s="36"/>
       <c r="O82" s="2"/>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83" s="2"/>
-      <c r="C83" s="38"/>
-      <c r="E83" s="38"/>
-      <c r="G83" s="38"/>
-      <c r="N83" s="39"/>
+      <c r="C83" s="35"/>
+      <c r="E83" s="35"/>
+      <c r="G83" s="35"/>
+      <c r="N83" s="36"/>
       <c r="O83" s="2"/>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B84" s="2"/>
-      <c r="C84" s="38"/>
-      <c r="E84" s="38"/>
-      <c r="G84" s="38"/>
-      <c r="N84" s="39"/>
+      <c r="C84" s="35"/>
+      <c r="E84" s="35"/>
+      <c r="G84" s="35"/>
+      <c r="N84" s="36"/>
       <c r="O84" s="2"/>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B85" s="2"/>
-      <c r="C85" s="38"/>
-      <c r="E85" s="38"/>
-      <c r="G85" s="38"/>
-      <c r="N85" s="39"/>
+      <c r="C85" s="35"/>
+      <c r="E85" s="35"/>
+      <c r="G85" s="35"/>
+      <c r="N85" s="36"/>
       <c r="O85" s="2"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B86" s="2"/>
-      <c r="C86" s="38"/>
-      <c r="E86" s="38"/>
-      <c r="G86" s="38"/>
-      <c r="N86" s="39"/>
+      <c r="C86" s="35"/>
+      <c r="E86" s="35"/>
+      <c r="G86" s="35"/>
+      <c r="N86" s="36"/>
       <c r="O86" s="2"/>
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87" s="2"/>
-      <c r="C87" s="38"/>
-      <c r="E87" s="38"/>
-      <c r="G87" s="38"/>
-      <c r="N87" s="39"/>
+      <c r="C87" s="35"/>
+      <c r="E87" s="35"/>
+      <c r="G87" s="35"/>
+      <c r="N87" s="36"/>
       <c r="O87" s="2"/>
     </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B88" s="2"/>
-      <c r="C88" s="38"/>
-      <c r="E88" s="38"/>
-      <c r="G88" s="38"/>
-      <c r="N88" s="39"/>
+      <c r="C88" s="35"/>
+      <c r="E88" s="35"/>
+      <c r="G88" s="35"/>
+      <c r="N88" s="36"/>
       <c r="O88" s="2"/>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B89" s="2"/>
-      <c r="C89" s="38"/>
-      <c r="E89" s="38"/>
-      <c r="G89" s="38"/>
-      <c r="N89" s="39"/>
+      <c r="C89" s="35"/>
+      <c r="E89" s="35"/>
+      <c r="G89" s="35"/>
+      <c r="N89" s="36"/>
       <c r="O89" s="2"/>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B90" s="2"/>
-      <c r="C90" s="38"/>
-      <c r="E90" s="38"/>
-      <c r="G90" s="38"/>
-      <c r="N90" s="39"/>
+      <c r="C90" s="35"/>
+      <c r="E90" s="35"/>
+      <c r="G90" s="35"/>
+      <c r="N90" s="36"/>
       <c r="O90" s="2"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B91" s="2"/>
-      <c r="C91" s="38"/>
-      <c r="E91" s="38"/>
-      <c r="G91" s="38"/>
-      <c r="N91" s="39"/>
+      <c r="C91" s="35"/>
+      <c r="E91" s="35"/>
+      <c r="G91" s="35"/>
+      <c r="N91" s="36"/>
       <c r="O91" s="2"/>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B92" s="2"/>
-      <c r="E92" s="38"/>
-      <c r="G92" s="38"/>
-      <c r="N92" s="39"/>
+      <c r="E92" s="35"/>
+      <c r="G92" s="35"/>
+      <c r="N92" s="36"/>
       <c r="O92" s="2"/>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B93" s="2"/>
-      <c r="E93" s="38"/>
-      <c r="G93" s="38"/>
-      <c r="N93" s="39"/>
+      <c r="E93" s="35"/>
+      <c r="G93" s="35"/>
+      <c r="N93" s="36"/>
       <c r="O93" s="2"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B94" s="2"/>
-      <c r="E94" s="38"/>
-      <c r="G94" s="38"/>
-      <c r="N94" s="39"/>
+      <c r="E94" s="35"/>
+      <c r="G94" s="35"/>
+      <c r="N94" s="36"/>
       <c r="O94" s="2"/>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B95" s="2"/>
-      <c r="E95" s="38"/>
-      <c r="G95" s="38"/>
-      <c r="N95" s="39"/>
+      <c r="E95" s="35"/>
+      <c r="G95" s="35"/>
+      <c r="N95" s="36"/>
       <c r="O95" s="2"/>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B96" s="2"/>
-      <c r="E96" s="38"/>
-      <c r="G96" s="38"/>
-      <c r="N96" s="39"/>
+      <c r="E96" s="35"/>
+      <c r="G96" s="35"/>
+      <c r="N96" s="36"/>
       <c r="O96" s="2"/>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B97" s="2"/>
-      <c r="E97" s="38"/>
-      <c r="G97" s="38"/>
-      <c r="N97" s="39"/>
+      <c r="E97" s="35"/>
+      <c r="G97" s="35"/>
+      <c r="N97" s="36"/>
       <c r="O97" s="2"/>
     </row>
     <row r="98" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B98" s="2"/>
-      <c r="E98" s="38"/>
-      <c r="G98" s="38"/>
-      <c r="N98" s="39"/>
+      <c r="E98" s="35"/>
+      <c r="G98" s="35"/>
+      <c r="N98" s="36"/>
       <c r="O98" s="2"/>
     </row>
     <row r="99" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B99" s="2"/>
-      <c r="E99" s="38"/>
-      <c r="G99" s="38"/>
-      <c r="N99" s="39"/>
+      <c r="E99" s="35"/>
+      <c r="G99" s="35"/>
+      <c r="N99" s="36"/>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B100" s="2"/>
-      <c r="E100" s="38"/>
-      <c r="G100" s="38"/>
-      <c r="N100" s="39"/>
+      <c r="E100" s="35"/>
+      <c r="G100" s="35"/>
+      <c r="N100" s="36"/>
     </row>
     <row r="101" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B101" s="2"/>
-      <c r="E101" s="38"/>
-      <c r="G101" s="38"/>
-      <c r="N101" s="39"/>
+      <c r="E101" s="35"/>
+      <c r="G101" s="35"/>
+      <c r="N101" s="36"/>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102" s="2"/>
-      <c r="E102" s="38"/>
-      <c r="G102" s="38"/>
-      <c r="N102" s="39"/>
+      <c r="E102" s="35"/>
+      <c r="G102" s="35"/>
+      <c r="N102" s="36"/>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B103" s="2"/>
-      <c r="E103" s="38"/>
-      <c r="G103" s="38"/>
-      <c r="N103" s="39"/>
+      <c r="E103" s="35"/>
+      <c r="G103" s="35"/>
+      <c r="N103" s="36"/>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104" s="2"/>
-      <c r="E104" s="38"/>
-      <c r="G104" s="38"/>
+      <c r="E104" s="35"/>
+      <c r="G104" s="35"/>
       <c r="N104" s="2"/>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B105" s="2"/>
-      <c r="E105" s="38"/>
-      <c r="G105" s="38"/>
+      <c r="E105" s="35"/>
+      <c r="G105" s="35"/>
       <c r="N105" s="2"/>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106" s="2"/>
-      <c r="E106" s="38"/>
-      <c r="G106" s="38"/>
+      <c r="E106" s="35"/>
+      <c r="G106" s="35"/>
       <c r="N106" s="2"/>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B107" s="2"/>
-      <c r="E107" s="38"/>
+      <c r="E107" s="35"/>
       <c r="N107" s="2"/>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B108" s="2"/>
-      <c r="E108" s="38"/>
+      <c r="E108" s="35"/>
       <c r="N108" s="2"/>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B109" s="2"/>
-      <c r="E109" s="38"/>
+      <c r="E109" s="35"/>
       <c r="N109" s="2"/>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B110" s="2"/>
-      <c r="E110" s="38"/>
+      <c r="E110" s="35"/>
       <c r="N110" s="2"/>
     </row>
   </sheetData>
@@ -11165,4 +11230,115 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40EC227C-CE34-4CA3-8A39-362F23C3DFAD}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="46" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="52">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="51" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" s="53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="51" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="51" t="s">
+        <v>244</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="51" t="s">
+        <v>246</v>
+      </c>
+      <c r="B7" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="51" t="s">
+        <v>247</v>
+      </c>
+      <c r="B8" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="51" t="s">
+        <v>248</v>
+      </c>
+      <c r="B9" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="B10" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="54"/>
+      <c r="B11" s="54"/>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="54"/>
+      <c r="B12" s="54"/>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="54"/>
+      <c r="B13" s="54"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>